<commit_message>
AOLM notes for code analysis/merging
</commit_message>
<xml_diff>
--- a/writings/notes/list_of_aolm_classes.xlsx
+++ b/writings/notes/list_of_aolm_classes.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Documents/school/aolm_full/writings/notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6F7400-DDBC-1743-8419-6FFCF0FE3331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D083AF-3A42-A347-B534-2C08F4A068CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" xr2:uid="{0A92EDB9-31E7-1A48-A805-0B106D93FACD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{0A92EDB9-31E7-1A48-A805-0B106D93FACD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$D$1:$D$48</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="126">
   <si>
     <t>class_name</t>
   </si>
@@ -356,6 +359,63 @@
   </si>
   <si>
     <t>metadata</t>
+  </si>
+  <si>
+    <t>kilgariff chi squared (authorship), read all texts into one string</t>
+  </si>
+  <si>
+    <t>read from file, tokenize (nltk)</t>
+  </si>
+  <si>
+    <t>read from file, tokenize (manual), remove stopwords (voyant)</t>
+  </si>
+  <si>
+    <t>read poems from bingham_bolts_of_melody</t>
+  </si>
+  <si>
+    <t>stores bolts poems by lines, sections</t>
+  </si>
+  <si>
+    <t>reads and stores a collection of DickinsonPoem objects, lexicon grepping, tf-idf</t>
+  </si>
+  <si>
+    <t>reads Gutenberg-formatted Dickinson poems into raw text</t>
+  </si>
+  <si>
+    <t>meant to be base DickinsonPoem reading class, frequency tallying and output, stanza retrieval, manual  tokenization, bow for collection, lexicon, title comparison, collection reading, poem comparison, line comparison, output by metadata filter functions</t>
+  </si>
+  <si>
+    <t>reads Dickinson correspondence xml, calculates line count, bow vector, metadata, stats, tag retrieval, lexicon, date functionality, text cleaning (manual), tokenization (manual)</t>
+  </si>
+  <si>
+    <t>Bare instance of DickinsonPoem class and gather_poems function for Emily Dickinson Archive</t>
+  </si>
+  <si>
+    <t>reads Dickinson poems from EDA format tei and turns into object, metadata, bow, bow vectors, line match, poem match, cleaning, conversion to plain text</t>
+  </si>
+  <si>
+    <t>Outputs book metadata from downloaded Hathitrust extracted features files</t>
+  </si>
+  <si>
+    <t>Reads in text file, cleans and tokenizes, calculates term frequencies</t>
+  </si>
+  <si>
+    <t>Calculates tf-idf vectors for all collection texts, outputs tf-idf to csv, and collection vocab to csv</t>
+  </si>
+  <si>
+    <t>Reads in a project gutenberg text using given reading method, separating raw text and text's main components, outputs text components into separate text files</t>
+  </si>
+  <si>
+    <t>HuckFinn child class of the project gutenberg text class from gutenberg_cleaning_dq. Includes file Huck Finn-specific component definition array, and component reading method for the object instantiation.</t>
+  </si>
+  <si>
+    <t>Text data quality metric comparison base class and Huck Finn-specific comparer class that has functions to compare different aspects of Huck Finn volumes. Includes stylometric and stat-tallying functions</t>
+  </si>
+  <si>
+    <t>Class GutenbergReader for re-ingesting (e.g. loading into memory) Gutenberg texts processed into separate component files by gutenberg_cleaning_dq.py</t>
+  </si>
+  <si>
+    <t>Read in Mark Twain Project Online tei files (i.e. Twain autobiography files) and retrieve tags and tag values from them</t>
   </si>
 </sst>
 </file>
@@ -504,10 +564,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -842,21 +901,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{830E0192-BDC1-3246-9617-241C6DCE7D37}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="214.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -876,750 +935,795 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:5" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:5" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:5" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:5" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:5" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:5" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
+    <row r="8" spans="1:5" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
+    <row r="9" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
+    <row r="10" spans="1:5" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="12" t="s">
+    <row r="11" spans="1:5" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="12" t="s">
+    <row r="12" spans="1:5" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="15" t="s">
+    <row r="13" spans="1:5" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="15" t="s">
+    <row r="14" spans="1:5" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="15" t="s">
+    <row r="15" spans="1:5" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="16" t="s">
+    <row r="16" spans="1:5" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="E16" s="16"/>
-    </row>
-    <row r="17" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="16" t="s">
+      <c r="E16" s="15"/>
+    </row>
+    <row r="17" spans="1:5" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="E17" s="16"/>
-    </row>
-    <row r="18" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="E17" s="15"/>
+    </row>
+    <row r="18" spans="1:5" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="9" t="s">
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="1:5" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="8" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="9" t="s">
+    <row r="21" spans="1:5" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="8" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="9" t="s">
+    <row r="22" spans="1:5" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E22" s="8" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="9" t="s">
+    <row r="23" spans="1:5" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="8" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="12" t="s">
+    <row r="24" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E24" s="12"/>
-    </row>
-    <row r="25" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="12" t="s">
+      <c r="E24" s="11"/>
+    </row>
+    <row r="25" spans="1:5" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E25" s="12"/>
-    </row>
-    <row r="26" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="13" t="s">
+      <c r="E25" s="11"/>
+    </row>
+    <row r="26" spans="1:5" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D26" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="E26" s="8" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="13" t="s">
+    <row r="27" spans="1:5" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E27" s="13"/>
-    </row>
-    <row r="28" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="16" t="s">
+      <c r="E27" s="12"/>
+    </row>
+    <row r="28" spans="1:5" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D28" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E28" s="16"/>
-    </row>
-    <row r="29" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="16" t="s">
+      <c r="E28" s="15"/>
+    </row>
+    <row r="29" spans="1:5" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="C29" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D29" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E29" s="16"/>
-    </row>
-    <row r="30" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
+      <c r="E29" s="15"/>
+    </row>
+    <row r="30" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E30" s="3"/>
-    </row>
-    <row r="31" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
+      <c r="D30" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E31" s="3"/>
-    </row>
-    <row r="32" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
+      <c r="D31" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E32" s="3"/>
-    </row>
-    <row r="33" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="5" t="s">
+      <c r="D32" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D33" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E33" s="5"/>
-    </row>
-    <row r="34" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="5" t="s">
+      <c r="D33" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D34" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E34" s="5"/>
-    </row>
-    <row r="35" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="6" t="s">
+      <c r="D34" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D35" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E35" s="6"/>
-    </row>
-    <row r="36" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="6" t="s">
+      <c r="D35" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D36" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E36" s="6"/>
-    </row>
-    <row r="37" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="6" t="s">
+      <c r="D36" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D37" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E37" s="6"/>
-    </row>
-    <row r="38" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="6" t="s">
+      <c r="D37" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D38" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E38" s="6"/>
-    </row>
-    <row r="39" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="7" t="s">
+      <c r="D38" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C39" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D39" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E39" s="7"/>
-    </row>
-    <row r="40" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="9" t="s">
+      <c r="D39" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="9" t="s">
+      <c r="C40" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D40" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E40" s="9"/>
-    </row>
-    <row r="41" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="8" t="s">
+      <c r="D40" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="B41" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="C41" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D41" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E41" s="8"/>
-    </row>
-    <row r="42" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="10" t="s">
+      <c r="D41" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C42" s="10" t="s">
+      <c r="C42" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D42" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E42" s="10"/>
-    </row>
-    <row r="43" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="10" t="s">
+      <c r="D42" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B43" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C43" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D43" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E43" s="10"/>
-    </row>
-    <row r="44" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="11" t="s">
+      <c r="D43" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B44" s="11" t="s">
+      <c r="B44" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C44" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D44" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E44" s="11"/>
-    </row>
-    <row r="45" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="11" t="s">
+      <c r="D44" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B45" s="11" t="s">
+      <c r="B45" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C45" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D45" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E45" s="11"/>
-    </row>
-    <row r="46" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="12" t="s">
+      <c r="D45" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B46" s="12" t="s">
+      <c r="B46" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="12" t="s">
+      <c r="C46" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D46" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E46" s="12"/>
-    </row>
-    <row r="47" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="12" t="s">
+      <c r="D46" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B47" s="12" t="s">
+      <c r="B47" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C47" s="12" t="s">
+      <c r="C47" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D47" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E47" s="12"/>
-    </row>
-    <row r="48" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="14" t="s">
+      <c r="D47" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C48" s="14" t="s">
+      <c r="C48" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D48" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E48" s="14"/>
+      <c r="D48" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E48" s="13" t="s">
+        <v>125</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="D1:D48" xr:uid="{830E0192-BDC1-3246-9617-241C6DCE7D37}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="text ingestion"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E48">
     <sortCondition ref="D2:D48"/>
   </sortState>

</xml_diff>